<commit_message>
updated ReadME and cleaned data
</commit_message>
<xml_diff>
--- a/cornell_shots.xlsx
+++ b/cornell_shots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlie/Data/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA34413-238B-DB41-BCAD-B8047332C7DE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189752CC-F000-2344-AD3E-FC9A695F751E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13560" yWindow="1340" windowWidth="13880" windowHeight="14180" xr2:uid="{AC1E0B3E-1B30-B948-ABC9-188344C1A5DC}"/>
   </bookViews>
@@ -104,7 +104,7 @@
     <t>Defensive Midfield</t>
   </si>
   <si>
-    <t>#17 - B.Bayh</t>
+    <t>#17 - B. Bayh</t>
   </si>
   <si>
     <t>#47 - B. Evans</t>
@@ -461,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B078861-BD03-3347-9263-3A4D9610AC3E}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>